<commit_message>
Added feature (Tooltips are shown on mouseover) anf Refoctoring
</commit_message>
<xml_diff>
--- a/scripts/Map.xlsx
+++ b/scripts/Map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="name_heroes" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,7 +13,8 @@
     <sheet name="base_heroes" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="base_skills" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="png_skills" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Sheet6" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Sheet7" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Sheet6" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">png_skills!$A$3:$A$361</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8383" uniqueCount="4103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8607" uniqueCount="4168">
   <si>
     <t xml:space="preserve">db_en</t>
   </si>
@@ -60,7 +61,7 @@
     <t xml:space="preserve">"name": "クロム",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Corrin(M)",</t>
+    <t xml:space="preserve">"name_en": "Corrin (M)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "カムイ(男)",</t>
@@ -138,7 +139,7 @@
     <t xml:space="preserve">"name": "リリーナ",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Lonqu",</t>
+    <t xml:space="preserve">"name_en": "Lon'qu",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "ロンク―",</t>
@@ -234,13 +235,13 @@
     <t xml:space="preserve">"name": "サーリャ",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Tiki(A)",</t>
+    <t xml:space="preserve">"name_en": "Tiki (Adult)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "チキ(大人)",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Tiki(Y)",</t>
+    <t xml:space="preserve">"name_en": "Tiki (Young)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "チキ(子供)",</t>
@@ -360,7 +361,7 @@
     <t xml:space="preserve">"name": "レイヴァン",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Robin(F)",</t>
+    <t xml:space="preserve">"name_en": "Robin (F)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "ルフレ(女)",</t>
@@ -396,7 +397,7 @@
     <t xml:space="preserve">"name": "ティアモ",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Corrin(F)",</t>
+    <t xml:space="preserve">"name_en": "Corrin (F)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "カムイ(女)",</t>
@@ -498,7 +499,7 @@
     <t xml:space="preserve">"name": "ラインハルト",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Robin(M)",</t>
+    <t xml:space="preserve">"name_en": "Robin (M)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "ルフレ(男)",</t>
@@ -696,25 +697,25 @@
     <t xml:space="preserve">"name": "ミシェイル",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Lucina (Spring)",</t>
+    <t xml:space="preserve">"name_en": "Lucina (Spring Festival)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "ルキナ(豊穣の春祭り)",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Camilla (Spring)",</t>
+    <t xml:space="preserve">"name_en": "Camilla (Spring Festival)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "カミラ(豊穣の春祭り)",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Xander (Spring)",</t>
+    <t xml:space="preserve">"name_en": "Xander (Spring Festival)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "マークス(豊穣の春祭り)",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Chrom (Spring)",</t>
+    <t xml:space="preserve">"name_en": "Chrom (Spring Festival)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "クロム(豊穣の春祭り)",</t>
@@ -816,7 +817,7 @@
     <t xml:space="preserve">"name": "ロイド",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Caeda (Bride)",</t>
+    <t xml:space="preserve">"name_en": "Caeda (Bridal Blessings)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "シーダ(花嫁たちに祝福を)",</t>
@@ -828,19 +829,19 @@
     <t xml:space="preserve">"name": "カミュ",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Charlotte (Bride)",</t>
+    <t xml:space="preserve">"name_en": "Charlotte (Bridal Blessings)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "シャーロッテ(花嫁たちに祝福を)",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Cordelia (Bride)",</t>
+    <t xml:space="preserve">"name_en": "Cordelia (Bridal Blessings)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "ティアモ(花嫁たちに祝福を)",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Lyn (Bride)",</t>
+    <t xml:space="preserve">"name_en": "Lyn (Bridal Blessings)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "リン(花嫁たちに祝福を)",</t>
@@ -888,25 +889,25 @@
     <t xml:space="preserve">"name": "クライネ",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Frederick (Summer)",</t>
+    <t xml:space="preserve">"name_en": "Frederick (Ylissean Summer)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "フレデリク(覚醒の夏)",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Gaius (Summer)",</t>
+    <t xml:space="preserve">"name_en": "Gaius (Ylissean Summer)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "ガイア(覚醒の夏)",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Robin(F) (Summer)",</t>
+    <t xml:space="preserve">"name_en": "Robin (F) (Ylissean Summer)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "ルフレ(女)(覚醒の夏)",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Tiki(A) (Summer)",</t>
+    <t xml:space="preserve">"name_en": "Tiki (Adult) (Ylissean Summer)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "チキ(大人)(覚醒の夏)",</t>
@@ -960,25 +961,25 @@
     <t xml:space="preserve">"name": "ベルクト",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Corrin(F) (Summer)",</t>
+    <t xml:space="preserve">"name_en": "Corrin (F) (Nohrian Summer)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "カムイ(女)(暗夜の夏)",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Leo (Summer)",</t>
+    <t xml:space="preserve">"name_en": "Leo (Nohrian Summer)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "レオン(暗夜の夏)",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Xander (Summer)",</t>
+    <t xml:space="preserve">"name_en": "Xander (Nohrian Summer)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "マークス(暗夜の夏)",</t>
   </si>
   <si>
-    <t xml:space="preserve">"name_en": "Elise (Summer)",</t>
+    <t xml:space="preserve">"name_en": "Elise (Nohrian Summer)",</t>
   </si>
   <si>
     <t xml:space="preserve">"name": "エリーゼ(暗夜の夏)",</t>
@@ -12274,6 +12275,201 @@
   </si>
   <si>
     <t xml:space="preserve">Wrathful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bruno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caeda (Bridal Blessings)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camilla (Spring Festival)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charlotte (Bridal Blessings)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chrom (Spring Festival)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cordelia (Bridal Blessings)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corrin (F) (Nohrian Summer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corrin (F)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corrin (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dorcas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elise (Nohrian Summer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fjorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frederick (Ylissean Summer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaius (Ylissean Summer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_armored_axe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_armored_lance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_armored_sword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_cavalry_axe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_cavalry_bluetome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_cavalry_bow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_cavalry_greentome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_cavalry_lance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_cavalry_redtome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_cavalry_staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_cavalry_sword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_flying_axe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_flying_lance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_flying_sword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_infantry_axe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_infantry_bluetome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_infantry_bow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_infantry_dagger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_infantry_greentome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_infantry_lance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_infantry_redtome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_infantry_staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic_infantry_sword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Henry (Trick or Defeat!)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Henry (Trick or Defeat)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jakob (Trick or Defeat!)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jakob (Trick or Defeat)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joshua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lævateinn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leo (Nohrian Summer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lon'qu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucina (Spring Festival)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lyn (Bridal Blessings)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nohero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nowi (Trick or Defeat!)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nowi (Trick or Defeat)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robin (F)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robin (F) (Ylissean Summer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robin (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sakura (Trick or Defeat!)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sakura (Trick or Defeat)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surtr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiki (Adult)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiki (Adult) (Ylissean Summer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiki (Young)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veronica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xander (Nohrian Summer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xander (Spring Festival)</t>
   </si>
   <si>
     <t xml:space="preserve">Effective against armored units</t>
@@ -12447,8 +12643,8 @@
   </sheetPr>
   <dimension ref="A1:B191"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A160" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A172" activeCellId="0" sqref="A172"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -51562,9 +51758,1157 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:A224"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A202" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D213" activeCellId="0" sqref="D213"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="9.33"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>1938</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>2056</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>2142</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>1896</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>2186</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>2188</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>2180</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>2170</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>2132</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>2168</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>4082</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>4083</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>4084</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>2088</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>1942</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>1908</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>4085</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>4086</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>2058</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>4087</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>4088</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>4089</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>4090</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>2182</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>4091</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>2162</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>4092</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>2062</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>4093</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>4094</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>4095</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>4097</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>4098</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>4101</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>4102</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>4103</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>4104</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>4105</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>4106</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>4107</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>4108</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>4109</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>4110</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>4111</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>4112</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>4113</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>4114</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>4115</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>4116</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>4117</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>4118</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>2124</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>4119</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>4120</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>2152</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>2066</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>2172</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>2144</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>4121</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>4122</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>4123</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>2098</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>4124</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>4125</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>2126</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>2084</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>4126</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>4127</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>2156</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>4128</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>2104</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>4129</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>2154</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>4130</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>2096</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>2130</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>4131</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>2068</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>1928</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>2054</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>4132</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>4133</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>4134</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>2174</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>1870</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>2166</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>1872</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>4135</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>4136</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>4137</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>2102</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>2158</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>4138</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>4139</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="s">
+        <v>1882</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="s">
+        <v>1884</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="s">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="s">
+        <v>2148</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>2176</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>2178</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
+        <v>2122</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>1886</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="s">
+        <v>2070</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="s">
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>2184</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
+        <v>2146</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="s">
+        <v>4141</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="s">
+        <v>4142</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>4143</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="s">
+        <v>2072</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="s">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>4144</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="s">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0" t="s">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="s">
+        <v>4145</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="0" t="s">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="0" t="s">
+        <v>4146</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="0" t="s">
+        <v>2064</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12ページ &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -51585,87 +52929,87 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4082</v>
+        <v>4147</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4083</v>
+        <v>4148</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4084</v>
+        <v>4149</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4085</v>
+        <v>4150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>4086</v>
+        <v>4151</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4087</v>
+        <v>4152</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>4088</v>
+        <v>4153</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4089</v>
+        <v>4154</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>4090</v>
+        <v>4155</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>4091</v>
+        <v>4156</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>4092</v>
+        <v>4157</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>4093</v>
+        <v>4158</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>4094</v>
+        <v>4159</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4095</v>
+        <v>4160</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>4096</v>
+        <v>4161</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>4097</v>
+        <v>4162</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>4098</v>
+        <v>4163</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>4099</v>
+        <v>4164</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>4100</v>
+        <v>4165</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>4101</v>
+        <v>4166</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>4102</v>
+        <v>4167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>